<commit_message>
Added further TCs Added parallel execution Added screenshot capture mechanism Added parameters
</commit_message>
<xml_diff>
--- a/mapsync/QITestCases.xlsx
+++ b/mapsync/QITestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rahul.chakrabort\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Eclipse\HomeTest\MapSyncTest\QI-MapSync\mapsync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD29F822-E5B1-4FD1-BC1C-238C6D4BBB08}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E034A73-B344-4C78-8F03-948424F306FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="10980" xr2:uid="{1F7419F7-5BC7-49B5-9022-88CE8525904F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="160">
   <si>
     <t>Modules</t>
   </si>
@@ -295,12 +295,6 @@
     <t>Tolls Listing</t>
   </si>
   <si>
-    <t>Register As New User from Shortcut Menu Link</t>
-  </si>
-  <si>
-    <t>Register as New user from Personal Tab</t>
-  </si>
-  <si>
     <t>Signin From Shortcut Menu Link</t>
   </si>
   <si>
@@ -320,6 +314,222 @@
   </si>
   <si>
     <t>Map Operations</t>
+  </si>
+  <si>
+    <t>Click on shortcut menu option Register</t>
+  </si>
+  <si>
+    <t>Registration Page is displayed</t>
+  </si>
+  <si>
+    <t>A valid error message is displayed</t>
+  </si>
+  <si>
+    <t>Enter data in optional field only, leave mandatory fields blank and click on Create Profile</t>
+  </si>
+  <si>
+    <t>Enter valid data in all mandatory fields, leave optional fields blank and click on Create Profile</t>
+  </si>
+  <si>
+    <t>No Error message should be displayed, profile should be created successfully</t>
+  </si>
+  <si>
+    <t>New Registration Validation - shortcut link</t>
+  </si>
+  <si>
+    <t>AU005_RegistrationValidation</t>
+  </si>
+  <si>
+    <t>TC009</t>
+  </si>
+  <si>
+    <t>Click on Tab Personal and Click on button Register</t>
+  </si>
+  <si>
+    <t>TC010</t>
+  </si>
+  <si>
+    <t>New Registration Validation - Personal Tab</t>
+  </si>
+  <si>
+    <t>Validate that incident tab is auto selected</t>
+  </si>
+  <si>
+    <t>incidents tab is auto selected</t>
+  </si>
+  <si>
+    <t>Validate that incidents icons are properly displayed on the map</t>
+  </si>
+  <si>
+    <t>icons are displayed on the map and are clickable</t>
+  </si>
+  <si>
+    <t>click on any of the incidents icon having multiple entries</t>
+  </si>
+  <si>
+    <t>click on any of the incidents icon having single entry</t>
+  </si>
+  <si>
+    <t>On Map Operation Validations - Incidents</t>
+  </si>
+  <si>
+    <t>popup with incident details is shown up and expected number of incidents details are also displayed and a Zoom In link is also displayed in the popup</t>
+  </si>
+  <si>
+    <t>click on the incident link displayed in the popup</t>
+  </si>
+  <si>
+    <t>the corresponding incident detail popup is displayed, map zoomed in, incident details matches</t>
+  </si>
+  <si>
+    <t>On Map Operation Validations - cameras</t>
+  </si>
+  <si>
+    <t>unselect incidents tab and select cameras tab</t>
+  </si>
+  <si>
+    <t>cameras tab can be selected</t>
+  </si>
+  <si>
+    <t>Validate that cameras icons are properly displayed on the map</t>
+  </si>
+  <si>
+    <t>click on any of the cameras icon having multiple entries</t>
+  </si>
+  <si>
+    <t>click on any of the cameras icon having single entry</t>
+  </si>
+  <si>
+    <t>popup with cameras details is shown up and expected number of cameras details are also displayed and a Zoom In link is also displayed in the popup</t>
+  </si>
+  <si>
+    <t>click on the cameras link displayed in the popup</t>
+  </si>
+  <si>
+    <t>the corresponding cameras detail popup is displayed, map zoomed in, cameras details matches</t>
+  </si>
+  <si>
+    <t>popup with cameras details is shown up and camera image is also displayed</t>
+  </si>
+  <si>
+    <t>popup with incident details is shown up and incidents type, location info are also displayed</t>
+  </si>
+  <si>
+    <t>On Map Operation Validations - tolls</t>
+  </si>
+  <si>
+    <t>unselect incidents tab and select tolls tab</t>
+  </si>
+  <si>
+    <t>tolls tab can be selected</t>
+  </si>
+  <si>
+    <t>Validate that tolls icons are properly displayed on the map</t>
+  </si>
+  <si>
+    <t>click on any of the tolls icon having multiple entries</t>
+  </si>
+  <si>
+    <t>popup with tolls details is shown up and expected number of tolls details are also displayed and a Zoom In link is also displayed in the popup</t>
+  </si>
+  <si>
+    <t>click on the tolls link displayed in the popup</t>
+  </si>
+  <si>
+    <t>the corresponding tolls detail popup is displayed, map zoomed in, tolls details matches</t>
+  </si>
+  <si>
+    <t>click on any of the tolls icon having single entry</t>
+  </si>
+  <si>
+    <t>popup with tolls details is shown up and tax rate table is also displayed</t>
+  </si>
+  <si>
+    <t>On Map Operation Validations - parking</t>
+  </si>
+  <si>
+    <t>unselect incidents tab and select parking tab</t>
+  </si>
+  <si>
+    <t>parking tab can be selected</t>
+  </si>
+  <si>
+    <t>Validate that parking icons are properly displayed on the map</t>
+  </si>
+  <si>
+    <t>click on any of the parking icon having multiple entries</t>
+  </si>
+  <si>
+    <t>popup with parking details is shown up and expected number of parking details are also displayed and a Zoom In link is also displayed in the popup</t>
+  </si>
+  <si>
+    <t>click on the parking link displayed in the popup</t>
+  </si>
+  <si>
+    <t>the corresponding parking detail popup is displayed, map zoomed in, parking details matches</t>
+  </si>
+  <si>
+    <t>click on any of the parking icon having single entry</t>
+  </si>
+  <si>
+    <t>popup with parking details is shown up and location details are matched</t>
+  </si>
+  <si>
+    <t>On Map Operation Validations - traffic</t>
+  </si>
+  <si>
+    <t>Validate that traffic icons are properly displayed on the map</t>
+  </si>
+  <si>
+    <t>click on any of the traffic icon having multiple entries</t>
+  </si>
+  <si>
+    <t>popup with traffic details is shown up and expected number of traffic details are also displayed and a Zoom In link is also displayed in the popup</t>
+  </si>
+  <si>
+    <t>click on the traffic link displayed in the popup</t>
+  </si>
+  <si>
+    <t>the corresponding traffic detail popup is displayed, map zoomed in, traffic details matches</t>
+  </si>
+  <si>
+    <t>click on any of the traffic icon having single entry</t>
+  </si>
+  <si>
+    <t>popup with traffic details is shown up and location details are matched</t>
+  </si>
+  <si>
+    <t>TC011</t>
+  </si>
+  <si>
+    <t>TC012</t>
+  </si>
+  <si>
+    <t>TC013</t>
+  </si>
+  <si>
+    <t>TC014</t>
+  </si>
+  <si>
+    <t>TC015</t>
+  </si>
+  <si>
+    <t>AU006_MapOperationValidationIncidents</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>AU007_MapOperationValidationCameras</t>
+  </si>
+  <si>
+    <t>AU008_MapOperationValidationTolls</t>
+  </si>
+  <si>
+    <t>AU009_MapOperationValidationParking</t>
+  </si>
+  <si>
+    <t>AU010_MapOperationValidationTraffic</t>
   </si>
 </sst>
 </file>
@@ -509,88 +719,88 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -915,16 +1125,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE891018-E7DC-4755-9363-596E6D5E37AB}">
-  <dimension ref="A1:F83"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F117" sqref="F117:F124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="55" style="1" customWidth="1"/>
     <col min="4" max="4" width="50.42578125" style="1" customWidth="1"/>
@@ -953,1001 +1163,1621 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>86</v>
+      <c r="F2" s="26" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="21"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="9"/>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="11"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="21"/>
+      <c r="B4" s="30"/>
       <c r="C4" s="9"/>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="8"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="9"/>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="11"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="23"/>
-      <c r="B6" s="8"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="9"/>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="24"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="15"/>
+      <c r="F7" s="28"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>87</v>
+      <c r="F8" s="12" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="26"/>
-      <c r="B9" s="18"/>
+      <c r="A9" s="24"/>
+      <c r="B9" s="15"/>
       <c r="C9" s="9"/>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="26"/>
-      <c r="B10" s="18"/>
+      <c r="A10" s="24"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="9"/>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="19"/>
+      <c r="F10" s="11"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="26"/>
-      <c r="B11" s="18"/>
+      <c r="A11" s="24"/>
+      <c r="B11" s="15"/>
       <c r="C11" s="9"/>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="19"/>
+      <c r="F11" s="11"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26"/>
-      <c r="B12" s="18"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="15"/>
       <c r="C12" s="9"/>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="9"/>
-      <c r="F12" s="19"/>
+      <c r="F12" s="11"/>
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="26"/>
-      <c r="B13" s="18"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="9"/>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="19"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="26"/>
-      <c r="B14" s="18"/>
+      <c r="A14" s="24"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="9"/>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="19"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="26"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14" t="s">
+      <c r="A15" s="24"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="21"/>
+      <c r="F15" s="13"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="24"/>
+      <c r="B16" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="17" t="s">
-        <v>87</v>
+      <c r="F16" s="12" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="18"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="15"/>
       <c r="C17" s="9"/>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="19"/>
+      <c r="F17" s="11"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="18"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="9"/>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="19"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="26"/>
-      <c r="B19" s="18"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="9"/>
-      <c r="D19" s="10" t="s">
+      <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="19"/>
+      <c r="F19" s="11"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="26"/>
-      <c r="B20" s="18"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="15"/>
       <c r="C20" s="9"/>
-      <c r="D20" s="10" t="s">
+      <c r="D20" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="9"/>
-      <c r="F20" s="19"/>
+      <c r="F20" s="11"/>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="26"/>
-      <c r="B21" s="18"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="15"/>
       <c r="C21" s="9"/>
-      <c r="D21" s="10" t="s">
+      <c r="D21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="11"/>
     </row>
     <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="18"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="15"/>
       <c r="C22" s="9"/>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="19"/>
+      <c r="F22" s="11"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="26"/>
-      <c r="B23" s="18"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="15"/>
       <c r="C23" s="9"/>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="11"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="27"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="14" t="s">
+      <c r="A24" s="25"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="21"/>
+      <c r="F24" s="13"/>
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="6" t="s">
+      <c r="E25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="29" t="s">
-        <v>88</v>
+      <c r="F25" s="17" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
-      <c r="B26" s="18"/>
+      <c r="B26" s="15"/>
       <c r="C26" s="9"/>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="30"/>
+      <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="33"/>
-      <c r="B27" s="18"/>
+      <c r="B27" s="15"/>
       <c r="C27" s="9"/>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="30"/>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
-      <c r="B28" s="18"/>
+      <c r="B28" s="15"/>
       <c r="C28" s="9"/>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F28" s="30"/>
+      <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="33"/>
-      <c r="B29" s="18"/>
+      <c r="B29" s="15"/>
       <c r="C29" s="9"/>
-      <c r="D29" s="10" t="s">
+      <c r="D29" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E29" s="9"/>
-      <c r="F29" s="30"/>
+      <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="33"/>
-      <c r="B30" s="18"/>
+      <c r="B30" s="15"/>
       <c r="C30" s="9"/>
-      <c r="D30" s="10" t="s">
+      <c r="D30" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="30"/>
+      <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="33"/>
-      <c r="B31" s="18"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="9"/>
-      <c r="D31" s="10" t="s">
+      <c r="D31" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="33"/>
-      <c r="B32" s="18"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="9"/>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E32" s="10" t="s">
+      <c r="E32" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F32" s="30"/>
+      <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="33"/>
-      <c r="B33" s="18"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="9"/>
-      <c r="D33" s="10" t="s">
+      <c r="D33" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E33" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="30"/>
+      <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="33"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="14" t="s">
+      <c r="B34" s="16"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F34" s="31"/>
+      <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="33"/>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="6" t="s">
+      <c r="D35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="17" t="s">
-        <v>88</v>
+      <c r="F35" s="12" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="33"/>
-      <c r="B36" s="18"/>
+      <c r="B36" s="15"/>
       <c r="C36" s="9"/>
-      <c r="D36" s="10" t="s">
+      <c r="D36" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E36" s="10" t="s">
+      <c r="E36" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="19"/>
+      <c r="F36" s="11"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="33"/>
-      <c r="B37" s="18"/>
+      <c r="B37" s="15"/>
       <c r="C37" s="9"/>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="19"/>
+      <c r="F37" s="11"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="33"/>
-      <c r="B38" s="18"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="9"/>
-      <c r="D38" s="10" t="s">
+      <c r="D38" s="5" t="s">
         <v>45</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F38" s="19"/>
+      <c r="F38" s="11"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="33"/>
-      <c r="B39" s="18"/>
+      <c r="B39" s="15"/>
       <c r="C39" s="9"/>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E39" s="9"/>
-      <c r="F39" s="19"/>
+      <c r="F39" s="11"/>
     </row>
     <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="33"/>
-      <c r="B40" s="18"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="9"/>
-      <c r="D40" s="10" t="s">
+      <c r="D40" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E40" s="28" t="s">
+      <c r="E40" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F40" s="19"/>
+      <c r="F40" s="11"/>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="33"/>
-      <c r="B41" s="18"/>
+      <c r="B41" s="15"/>
       <c r="C41" s="9"/>
-      <c r="D41" s="10" t="s">
+      <c r="D41" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="19"/>
+      <c r="F41" s="11"/>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="33"/>
-      <c r="B42" s="18"/>
+      <c r="B42" s="15"/>
       <c r="C42" s="9"/>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="10" t="s">
+      <c r="E42" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F42" s="19"/>
+      <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="33"/>
-      <c r="B43" s="18"/>
+      <c r="B43" s="15"/>
       <c r="C43" s="9"/>
-      <c r="D43" s="10" t="s">
+      <c r="D43" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E43" s="10" t="s">
+      <c r="E43" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F43" s="19"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="33"/>
-      <c r="B44" s="18"/>
+      <c r="B44" s="15"/>
       <c r="C44" s="9"/>
-      <c r="D44" s="10" t="s">
+      <c r="D44" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E44" s="10" t="s">
+      <c r="E44" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F44" s="19"/>
+      <c r="F44" s="11"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="34"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="14" t="s">
+      <c r="B45" s="16"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F45" s="21"/>
+      <c r="F45" s="13"/>
     </row>
     <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E46" s="6" t="s">
+      <c r="E46" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F46" s="29" t="s">
+      <c r="F46" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="B47" s="18"/>
+      <c r="A47" s="11"/>
+      <c r="B47" s="15"/>
       <c r="C47" s="9"/>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="10" t="s">
+      <c r="E47" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F47" s="30"/>
+      <c r="F47" s="18"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="19"/>
-      <c r="B48" s="18"/>
+      <c r="A48" s="11"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="9"/>
-      <c r="D48" s="10" t="s">
+      <c r="D48" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F48" s="30"/>
+      <c r="F48" s="18"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="19"/>
-      <c r="B49" s="18"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="9"/>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E49" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F49" s="30"/>
+      <c r="F49" s="18"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="19"/>
-      <c r="B50" s="18"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="15"/>
       <c r="C50" s="9"/>
-      <c r="D50" s="10" t="s">
+      <c r="D50" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E50" s="9"/>
-      <c r="F50" s="30"/>
+      <c r="F50" s="18"/>
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="19"/>
-      <c r="B51" s="18"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="15"/>
       <c r="C51" s="9"/>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E51" s="10" t="s">
+      <c r="E51" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F51" s="30"/>
+      <c r="F51" s="18"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
-      <c r="B52" s="18"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="15"/>
       <c r="C52" s="9"/>
-      <c r="D52" s="10" t="s">
+      <c r="D52" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E52" s="10" t="s">
+      <c r="E52" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F52" s="30"/>
+      <c r="F52" s="18"/>
     </row>
     <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="19"/>
-      <c r="B53" s="18"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="15"/>
       <c r="C53" s="9"/>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E53" s="10" t="s">
+      <c r="E53" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F53" s="30"/>
+      <c r="F53" s="18"/>
     </row>
     <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
-      <c r="B54" s="18"/>
+      <c r="A54" s="11"/>
+      <c r="B54" s="15"/>
       <c r="C54" s="9"/>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E54" s="10" t="s">
+      <c r="E54" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F54" s="30"/>
+      <c r="F54" s="18"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="19"/>
-      <c r="B55" s="20"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="14" t="s">
+      <c r="A55" s="11"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E55" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F55" s="31"/>
+      <c r="F55" s="19"/>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="19"/>
-      <c r="B56" s="16" t="s">
+      <c r="A56" s="11"/>
+      <c r="B56" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D56" s="6" t="s">
+      <c r="D56" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E56" s="6" t="s">
+      <c r="E56" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F56" s="29" t="s">
+      <c r="F56" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="19"/>
-      <c r="B57" s="18"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="15"/>
       <c r="C57" s="9"/>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E57" s="10" t="s">
+      <c r="E57" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F57" s="30"/>
+      <c r="F57" s="18"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="19"/>
-      <c r="B58" s="18"/>
+      <c r="A58" s="11"/>
+      <c r="B58" s="15"/>
       <c r="C58" s="9"/>
-      <c r="D58" s="10" t="s">
+      <c r="D58" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E58" s="10" t="s">
+      <c r="E58" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F58" s="30"/>
+      <c r="F58" s="18"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="18"/>
+      <c r="A59" s="11"/>
+      <c r="B59" s="15"/>
       <c r="C59" s="9"/>
-      <c r="D59" s="10" t="s">
+      <c r="D59" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E59" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F59" s="30"/>
+      <c r="F59" s="18"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="19"/>
-      <c r="B60" s="18"/>
+      <c r="A60" s="11"/>
+      <c r="B60" s="15"/>
       <c r="C60" s="9"/>
-      <c r="D60" s="10" t="s">
+      <c r="D60" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E60" s="9"/>
-      <c r="F60" s="30"/>
+      <c r="F60" s="18"/>
     </row>
     <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="19"/>
-      <c r="B61" s="18"/>
+      <c r="A61" s="11"/>
+      <c r="B61" s="15"/>
       <c r="C61" s="9"/>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="E61" s="28" t="s">
+      <c r="E61" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F61" s="30"/>
+      <c r="F61" s="18"/>
     </row>
     <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="19"/>
-      <c r="B62" s="18"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="15"/>
       <c r="C62" s="9"/>
-      <c r="D62" s="10" t="s">
+      <c r="D62" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="E62" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F62" s="30"/>
+      <c r="F62" s="18"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="19"/>
-      <c r="B63" s="18"/>
+      <c r="A63" s="11"/>
+      <c r="B63" s="15"/>
       <c r="C63" s="9"/>
-      <c r="D63" s="10" t="s">
+      <c r="D63" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E63" s="10" t="s">
+      <c r="E63" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F63" s="30"/>
+      <c r="F63" s="18"/>
     </row>
     <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="19"/>
-      <c r="B64" s="18"/>
+      <c r="A64" s="11"/>
+      <c r="B64" s="15"/>
       <c r="C64" s="9"/>
-      <c r="D64" s="10" t="s">
+      <c r="D64" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E64" s="10" t="s">
+      <c r="E64" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F64" s="30"/>
+      <c r="F64" s="18"/>
     </row>
     <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="19"/>
-      <c r="B65" s="18"/>
+      <c r="A65" s="11"/>
+      <c r="B65" s="15"/>
       <c r="C65" s="9"/>
-      <c r="D65" s="10" t="s">
+      <c r="D65" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E65" s="10" t="s">
+      <c r="E65" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F65" s="30"/>
+      <c r="F65" s="18"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="19"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="14" t="s">
+      <c r="A66" s="11"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="E66" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F66" s="31"/>
+      <c r="F66" s="19"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="19"/>
-      <c r="B67" s="16" t="s">
+      <c r="A67" s="11"/>
+      <c r="B67" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="D67" s="6" t="s">
+      <c r="D67" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="E67" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F67" s="29" t="s">
+      <c r="F67" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="19"/>
-      <c r="B68" s="18"/>
+      <c r="A68" s="11"/>
+      <c r="B68" s="15"/>
       <c r="C68" s="9"/>
-      <c r="D68" s="10" t="s">
+      <c r="D68" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E68" s="10" t="s">
+      <c r="E68" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F68" s="30"/>
+      <c r="F68" s="18"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
-      <c r="B69" s="18"/>
+      <c r="A69" s="11"/>
+      <c r="B69" s="15"/>
       <c r="C69" s="9"/>
-      <c r="D69" s="10" t="s">
+      <c r="D69" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E69" s="10" t="s">
+      <c r="E69" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F69" s="30"/>
+      <c r="F69" s="18"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="19"/>
-      <c r="B70" s="18"/>
+      <c r="A70" s="11"/>
+      <c r="B70" s="15"/>
       <c r="C70" s="9"/>
-      <c r="D70" s="10" t="s">
+      <c r="D70" s="5" t="s">
         <v>61</v>
       </c>
       <c r="E70" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F70" s="30"/>
+      <c r="F70" s="18"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="19"/>
-      <c r="B71" s="18"/>
+      <c r="A71" s="11"/>
+      <c r="B71" s="15"/>
       <c r="C71" s="9"/>
-      <c r="D71" s="10" t="s">
+      <c r="D71" s="5" t="s">
         <v>62</v>
       </c>
       <c r="E71" s="9"/>
-      <c r="F71" s="30"/>
+      <c r="F71" s="18"/>
     </row>
     <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="19"/>
-      <c r="B72" s="18"/>
+      <c r="A72" s="11"/>
+      <c r="B72" s="15"/>
       <c r="C72" s="9"/>
-      <c r="D72" s="10" t="s">
+      <c r="D72" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E72" s="28" t="s">
+      <c r="E72" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F72" s="30"/>
+      <c r="F72" s="18"/>
     </row>
     <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="19"/>
-      <c r="B73" s="18"/>
+      <c r="A73" s="11"/>
+      <c r="B73" s="15"/>
       <c r="C73" s="9"/>
-      <c r="D73" s="10" t="s">
+      <c r="D73" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E73" s="10" t="s">
+      <c r="E73" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F73" s="30"/>
+      <c r="F73" s="18"/>
     </row>
     <row r="74" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A74" s="19"/>
-      <c r="B74" s="18"/>
+      <c r="A74" s="11"/>
+      <c r="B74" s="15"/>
       <c r="C74" s="9"/>
-      <c r="D74" s="10" t="s">
+      <c r="D74" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E74" s="10" t="s">
+      <c r="E74" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="F74" s="30"/>
+      <c r="F74" s="18"/>
     </row>
     <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="19"/>
-      <c r="B75" s="18"/>
+      <c r="A75" s="11"/>
+      <c r="B75" s="15"/>
       <c r="C75" s="9"/>
-      <c r="D75" s="10" t="s">
+      <c r="D75" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E75" s="10" t="s">
+      <c r="E75" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="F75" s="30"/>
+      <c r="F75" s="18"/>
     </row>
     <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="19"/>
-      <c r="B76" s="18"/>
+      <c r="A76" s="11"/>
+      <c r="B76" s="15"/>
       <c r="C76" s="9"/>
-      <c r="D76" s="10" t="s">
+      <c r="D76" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E76" s="10" t="s">
+      <c r="E76" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F76" s="30"/>
+      <c r="F76" s="18"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="19"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="13"/>
-      <c r="D77" s="14" t="s">
+      <c r="A77" s="11"/>
+      <c r="B77" s="16"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E77" s="14" t="s">
+      <c r="E77" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F77" s="31"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C78" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C79" s="1" t="s">
-        <v>82</v>
-      </c>
+      <c r="F77" s="19"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C80" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C81" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C82" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C81" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C82" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C83" s="1" t="s">
+    <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B84" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F84" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="11"/>
+      <c r="B85" s="15"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F85" s="18"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="11"/>
+      <c r="B86" s="15"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E86" s="5" t="s">
         <v>89</v>
       </c>
+      <c r="F86" s="18"/>
+    </row>
+    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="11"/>
+      <c r="B87" s="15"/>
+      <c r="C87" s="9"/>
+      <c r="D87" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F87" s="18"/>
+    </row>
+    <row r="88" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="11"/>
+      <c r="B88" s="16"/>
+      <c r="C88" s="10"/>
+      <c r="D88" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F88" s="19"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="11"/>
+      <c r="B89" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F89" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="11"/>
+      <c r="B90" s="15"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E90" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F90" s="18"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="11"/>
+      <c r="B91" s="15"/>
+      <c r="C91" s="9"/>
+      <c r="D91" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E91" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F91" s="18"/>
+    </row>
+    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="11"/>
+      <c r="B92" s="15"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F92" s="18"/>
+    </row>
+    <row r="93" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="11"/>
+      <c r="B93" s="16"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F93" s="19"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="C94" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F94" s="12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="11"/>
+      <c r="B95" s="15"/>
+      <c r="C95" s="9"/>
+      <c r="D95" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F95" s="11"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="11"/>
+      <c r="B96" s="15"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F96" s="11"/>
+    </row>
+    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="11"/>
+      <c r="B97" s="15"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F97" s="11"/>
+    </row>
+    <row r="98" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A98" s="11"/>
+      <c r="B98" s="15"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F98" s="11"/>
+    </row>
+    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A99" s="11"/>
+      <c r="B99" s="15"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F99" s="11"/>
+    </row>
+    <row r="100" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="11"/>
+      <c r="B100" s="16"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F100" s="13"/>
+    </row>
+    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="11"/>
+      <c r="B101" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F101" s="12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="11"/>
+      <c r="B102" s="15"/>
+      <c r="C102" s="9"/>
+      <c r="D102" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E102" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F102" s="11"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="11"/>
+      <c r="B103" s="15"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E103" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F103" s="11"/>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="11"/>
+      <c r="B104" s="15"/>
+      <c r="C104" s="9"/>
+      <c r="D104" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F104" s="11"/>
+    </row>
+    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A105" s="11"/>
+      <c r="B105" s="15"/>
+      <c r="C105" s="9"/>
+      <c r="D105" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F105" s="11"/>
+    </row>
+    <row r="106" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A106" s="11"/>
+      <c r="B106" s="15"/>
+      <c r="C106" s="9"/>
+      <c r="D106" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F106" s="11"/>
+    </row>
+    <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A107" s="11"/>
+      <c r="B107" s="15"/>
+      <c r="C107" s="9"/>
+      <c r="D107" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F107" s="11"/>
+    </row>
+    <row r="108" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="11"/>
+      <c r="B108" s="16"/>
+      <c r="C108" s="10"/>
+      <c r="D108" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="F108" s="13"/>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="11"/>
+      <c r="B109" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C109" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F109" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="11"/>
+      <c r="B110" s="15"/>
+      <c r="C110" s="9"/>
+      <c r="D110" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E110" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F110" s="11"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="11"/>
+      <c r="B111" s="15"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E111" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F111" s="11"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="11"/>
+      <c r="B112" s="15"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E112" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F112" s="11"/>
+    </row>
+    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="11"/>
+      <c r="B113" s="15"/>
+      <c r="C113" s="9"/>
+      <c r="D113" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F113" s="11"/>
+    </row>
+    <row r="114" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A114" s="11"/>
+      <c r="B114" s="15"/>
+      <c r="C114" s="9"/>
+      <c r="D114" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F114" s="11"/>
+    </row>
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="11"/>
+      <c r="B115" s="15"/>
+      <c r="C115" s="9"/>
+      <c r="D115" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E115" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F115" s="11"/>
+    </row>
+    <row r="116" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="11"/>
+      <c r="B116" s="16"/>
+      <c r="C116" s="10"/>
+      <c r="D116" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F116" s="13"/>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="11"/>
+      <c r="B117" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C117" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E117" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F117" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="11"/>
+      <c r="B118" s="15"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E118" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F118" s="11"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="11"/>
+      <c r="B119" s="15"/>
+      <c r="C119" s="9"/>
+      <c r="D119" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E119" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F119" s="11"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="11"/>
+      <c r="B120" s="15"/>
+      <c r="C120" s="9"/>
+      <c r="D120" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E120" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F120" s="11"/>
+    </row>
+    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A121" s="11"/>
+      <c r="B121" s="15"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F121" s="11"/>
+    </row>
+    <row r="122" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A122" s="11"/>
+      <c r="B122" s="15"/>
+      <c r="C122" s="9"/>
+      <c r="D122" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F122" s="11"/>
+    </row>
+    <row r="123" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A123" s="11"/>
+      <c r="B123" s="15"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E123" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F123" s="11"/>
+    </row>
+    <row r="124" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="11"/>
+      <c r="B124" s="16"/>
+      <c r="C124" s="10"/>
+      <c r="D124" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="F124" s="13"/>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="11"/>
+      <c r="B125" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C125" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F125" s="12" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="11"/>
+      <c r="B126" s="15"/>
+      <c r="C126" s="9"/>
+      <c r="D126" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E126" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F126" s="11"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="11"/>
+      <c r="B127" s="15"/>
+      <c r="C127" s="9"/>
+      <c r="D127" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E127" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F127" s="11"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="11"/>
+      <c r="B128" s="15"/>
+      <c r="C128" s="9"/>
+      <c r="D128" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E128" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F128" s="11"/>
+    </row>
+    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="11"/>
+      <c r="B129" s="15"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F129" s="11"/>
+    </row>
+    <row r="130" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A130" s="11"/>
+      <c r="B130" s="15"/>
+      <c r="C130" s="9"/>
+      <c r="D130" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F130" s="11"/>
+    </row>
+    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A131" s="11"/>
+      <c r="B131" s="15"/>
+      <c r="C131" s="9"/>
+      <c r="D131" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E131" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F131" s="11"/>
+    </row>
+    <row r="132" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="11"/>
+      <c r="B132" s="16"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F132" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F67:F77"/>
-    <mergeCell ref="C67:C77"/>
-    <mergeCell ref="B67:B77"/>
-    <mergeCell ref="A46:A77"/>
+  <mergeCells count="58">
     <mergeCell ref="A25:A45"/>
     <mergeCell ref="E49:E50"/>
     <mergeCell ref="B46:B55"/>
     <mergeCell ref="C46:C55"/>
     <mergeCell ref="F46:F55"/>
+    <mergeCell ref="B35:B45"/>
+    <mergeCell ref="C35:C45"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F35:F45"/>
+    <mergeCell ref="A46:A77"/>
     <mergeCell ref="E59:E60"/>
     <mergeCell ref="F56:F66"/>
     <mergeCell ref="C56:C66"/>
@@ -1957,10 +2787,6 @@
     <mergeCell ref="F25:F34"/>
     <mergeCell ref="C25:C34"/>
     <mergeCell ref="B25:B34"/>
-    <mergeCell ref="B35:B45"/>
-    <mergeCell ref="C35:C45"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F35:F45"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F16:F24"/>
     <mergeCell ref="C16:C24"/>
@@ -1972,7 +2798,34 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F8:F15"/>
     <mergeCell ref="C8:C15"/>
+    <mergeCell ref="B125:B132"/>
     <mergeCell ref="B8:B15"/>
+    <mergeCell ref="F84:F88"/>
+    <mergeCell ref="C84:C88"/>
+    <mergeCell ref="B84:B88"/>
+    <mergeCell ref="F89:F93"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="C89:C93"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F67:F77"/>
+    <mergeCell ref="C67:C77"/>
+    <mergeCell ref="B67:B77"/>
+    <mergeCell ref="C94:C100"/>
+    <mergeCell ref="A84:A93"/>
+    <mergeCell ref="A94:A132"/>
+    <mergeCell ref="F125:F132"/>
+    <mergeCell ref="C125:C132"/>
+    <mergeCell ref="C117:C124"/>
+    <mergeCell ref="C109:C116"/>
+    <mergeCell ref="C101:C108"/>
+    <mergeCell ref="F94:F100"/>
+    <mergeCell ref="F101:F108"/>
+    <mergeCell ref="F109:F116"/>
+    <mergeCell ref="F117:F124"/>
+    <mergeCell ref="B94:B100"/>
+    <mergeCell ref="B101:B108"/>
+    <mergeCell ref="B109:B116"/>
+    <mergeCell ref="B117:B124"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Test Case for Sign In Added new scripts Minor Refactoring Added Command Line Executor
</commit_message>
<xml_diff>
--- a/mapsync/QITestCases.xlsx
+++ b/mapsync/QITestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Eclipse\HomeTest\MapSyncTest\QI-MapSync\mapsync\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78691F59-5526-4FF2-B2C9-A461C80B0FDB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72484DD-29BE-4E7A-94BD-73F42F5894FD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="20610" windowHeight="10980" xr2:uid="{1F7419F7-5BC7-49B5-9022-88CE8525904F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="170">
   <si>
     <t>Modules</t>
   </si>
@@ -295,15 +295,6 @@
     <t>Tolls Listing</t>
   </si>
   <si>
-    <t>Signin From Shortcut Menu Link</t>
-  </si>
-  <si>
-    <t>Signin from Personal Tab</t>
-  </si>
-  <si>
-    <t>Other Shortcut Links</t>
-  </si>
-  <si>
     <t>AU001_Uivalidation</t>
   </si>
   <si>
@@ -530,6 +521,45 @@
   </si>
   <si>
     <t>AU010_MapOperationValidationTraffic</t>
+  </si>
+  <si>
+    <t>Sign In Validation - Shortcut Link</t>
+  </si>
+  <si>
+    <t>Click on link Sign In shortcut link</t>
+  </si>
+  <si>
+    <t>Sign In Page is displayed</t>
+  </si>
+  <si>
+    <t>enter any user name and password and click on button sign in</t>
+  </si>
+  <si>
+    <t>user should be signed in successfully and will ba landed onto my profile page</t>
+  </si>
+  <si>
+    <t>validate that no error message is displayed</t>
+  </si>
+  <si>
+    <t>no error message is displayed</t>
+  </si>
+  <si>
+    <t>Sign In Validation - Personal Tab</t>
+  </si>
+  <si>
+    <t>Click on tab Personal and Click on button Signin</t>
+  </si>
+  <si>
+    <t>TC016</t>
+  </si>
+  <si>
+    <t>TC017</t>
+  </si>
+  <si>
+    <t>AU011_SignInValidation</t>
+  </si>
+  <si>
+    <t>Sign IN</t>
   </si>
 </sst>
 </file>
@@ -709,7 +739,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -730,22 +760,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -757,6 +781,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -764,6 +794,15 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -784,15 +823,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -801,15 +831,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1125,11 +1146,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE891018-E7DC-4755-9363-596E6D5E37AB}">
-  <dimension ref="A1:F132"/>
+  <dimension ref="A1:F136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D87" sqref="D87"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1139,7 +1160,7 @@
     <col min="3" max="3" width="55" style="1" customWidth="1"/>
     <col min="4" max="4" width="50.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1163,13 +1184,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1178,78 +1199,78 @@
       <c r="E2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="26" t="s">
-        <v>84</v>
+      <c r="F2" s="20" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
+      <c r="A3" s="24"/>
       <c r="B3" s="30"/>
-      <c r="C3" s="9"/>
+      <c r="C3" s="11"/>
       <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="27"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="30"/>
-      <c r="C4" s="9"/>
+      <c r="C4" s="11"/>
       <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="27"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="30"/>
-      <c r="C5" s="9"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="30"/>
-      <c r="C6" s="9"/>
+      <c r="C6" s="11"/>
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="27"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="31"/>
-      <c r="C7" s="10"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="22"/>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="15" t="s">
         <v>34</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -1258,98 +1279,98 @@
       <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="12" t="s">
-        <v>85</v>
+      <c r="F8" s="20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="24"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="9"/>
+      <c r="A9" s="27"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="11"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="24"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="9"/>
+      <c r="A10" s="27"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="11"/>
       <c r="D10" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="9"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="24"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="9"/>
+      <c r="A12" s="27"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="11"/>
       <c r="D12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="9"/>
+      <c r="A13" s="27"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="5" t="s">
         <v>27</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F13" s="11"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="27"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="11"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="10"/>
+      <c r="A15" s="27"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="13"/>
+      <c r="F15" s="22"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="24"/>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="27"/>
+      <c r="B16" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -1358,112 +1379,112 @@
       <c r="E16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>85</v>
+      <c r="F16" s="20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="9"/>
+      <c r="A17" s="27"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="11"/>
       <c r="D17" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="11"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="24"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="9"/>
+      <c r="A18" s="27"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="11"/>
       <c r="D18" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="11"/>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="9"/>
+      <c r="A19" s="27"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="11"/>
       <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="11"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="24"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="9"/>
+      <c r="A20" s="27"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="24"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="9"/>
+      <c r="A21" s="27"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="5" t="s">
         <v>40</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F21" s="11"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="24"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="9"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="5" t="s">
         <v>42</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="11"/>
+      <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="24"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="9"/>
+      <c r="A23" s="27"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F23" s="11"/>
+      <c r="F23" s="21"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="25"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="10"/>
+      <c r="A24" s="28"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="16"/>
       <c r="D24" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="13"/>
+      <c r="F24" s="22"/>
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="32" t="s">
+      <c r="A25" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="15" t="s">
         <v>60</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -1473,13 +1494,13 @@
         <v>28</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="9"/>
+      <c r="A26" s="9"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="5" t="s">
         <v>23</v>
       </c>
@@ -1489,9 +1510,9 @@
       <c r="F26" s="18"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="33"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="9"/>
+      <c r="A27" s="9"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="5" t="s">
         <v>24</v>
       </c>
@@ -1501,31 +1522,31 @@
       <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="33"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="9"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E28" s="11" t="s">
         <v>47</v>
       </c>
       <c r="F28" s="18"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="33"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="9"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="11"/>
       <c r="D29" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="9"/>
+      <c r="E29" s="11"/>
       <c r="F29" s="18"/>
     </row>
     <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="33"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="9"/>
+      <c r="A30" s="9"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="11"/>
       <c r="D30" s="5" t="s">
         <v>55</v>
       </c>
@@ -1535,9 +1556,9 @@
       <c r="F30" s="18"/>
     </row>
     <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="33"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="9"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="11"/>
       <c r="D31" s="5" t="s">
         <v>49</v>
       </c>
@@ -1547,9 +1568,9 @@
       <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="33"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="9"/>
+      <c r="A32" s="9"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="11"/>
       <c r="D32" s="5" t="s">
         <v>51</v>
       </c>
@@ -1559,9 +1580,9 @@
       <c r="F32" s="18"/>
     </row>
     <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="9"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="11"/>
       <c r="D33" s="5" t="s">
         <v>35</v>
       </c>
@@ -1571,9 +1592,9 @@
       <c r="F33" s="18"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="33"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="10"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="16"/>
       <c r="D34" s="6" t="s">
         <v>37</v>
       </c>
@@ -1583,11 +1604,11 @@
       <c r="F34" s="19"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="33"/>
-      <c r="B35" s="14" t="s">
+      <c r="A35" s="9"/>
+      <c r="B35" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="15" t="s">
         <v>54</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -1596,136 +1617,136 @@
       <c r="E35" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F35" s="12" t="s">
-        <v>86</v>
+      <c r="F35" s="20" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="33"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="9"/>
+      <c r="A36" s="9"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="11"/>
       <c r="D36" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="11"/>
+      <c r="F36" s="21"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="33"/>
-      <c r="B37" s="15"/>
-      <c r="C37" s="9"/>
+      <c r="A37" s="9"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="11"/>
       <c r="D37" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F37" s="11"/>
+      <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="33"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="9"/>
+      <c r="A38" s="9"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="11"/>
       <c r="D38" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F38" s="11"/>
+      <c r="F38" s="21"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="33"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="9"/>
+      <c r="A39" s="9"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="11"/>
       <c r="D39" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="9"/>
-      <c r="F39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="21"/>
     </row>
     <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="9"/>
+      <c r="A40" s="9"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F40" s="11"/>
+      <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="9"/>
+      <c r="A41" s="9"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="11"/>
       <c r="D41" s="5" t="s">
         <v>57</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="11"/>
+      <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="33"/>
-      <c r="B42" s="15"/>
-      <c r="C42" s="9"/>
+      <c r="A42" s="9"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="11"/>
       <c r="D42" s="5" t="s">
         <v>49</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F42" s="11"/>
+      <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="33"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="9"/>
+      <c r="A43" s="9"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="11"/>
       <c r="D43" s="5" t="s">
         <v>51</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="F43" s="11"/>
+      <c r="F43" s="21"/>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="33"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="9"/>
+      <c r="A44" s="9"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="11"/>
       <c r="D44" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F44" s="11"/>
+      <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="34"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="10"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="16"/>
       <c r="D45" s="6" t="s">
         <v>37</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F45" s="13"/>
+      <c r="F45" s="22"/>
     </row>
     <row r="46" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="12" t="s">
+      <c r="A46" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="15" t="s">
         <v>59</v>
       </c>
       <c r="D46" s="4" t="s">
@@ -1739,9 +1760,9 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="11"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="9"/>
+      <c r="A47" s="21"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="11"/>
       <c r="D47" s="5" t="s">
         <v>23</v>
       </c>
@@ -1751,9 +1772,9 @@
       <c r="F47" s="18"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="11"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="9"/>
+      <c r="A48" s="21"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="11"/>
       <c r="D48" s="5" t="s">
         <v>24</v>
       </c>
@@ -1763,31 +1784,31 @@
       <c r="F48" s="18"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
-      <c r="B49" s="15"/>
-      <c r="C49" s="9"/>
+      <c r="A49" s="21"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="11"/>
       <c r="D49" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E49" s="11" t="s">
         <v>63</v>
       </c>
       <c r="F49" s="18"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="11"/>
-      <c r="B50" s="15"/>
-      <c r="C50" s="9"/>
+      <c r="A50" s="21"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="11"/>
       <c r="D50" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E50" s="9"/>
+      <c r="E50" s="11"/>
       <c r="F50" s="18"/>
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="11"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="9"/>
+      <c r="A51" s="21"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="11"/>
       <c r="D51" s="5" t="s">
         <v>64</v>
       </c>
@@ -1797,9 +1818,9 @@
       <c r="F51" s="18"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="11"/>
-      <c r="B52" s="15"/>
-      <c r="C52" s="9"/>
+      <c r="A52" s="21"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="11"/>
       <c r="D52" s="5" t="s">
         <v>65</v>
       </c>
@@ -1809,9 +1830,9 @@
       <c r="F52" s="18"/>
     </row>
     <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="11"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="9"/>
+      <c r="A53" s="21"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="11"/>
       <c r="D53" s="5" t="s">
         <v>67</v>
       </c>
@@ -1821,9 +1842,9 @@
       <c r="F53" s="18"/>
     </row>
     <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="11"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="9"/>
+      <c r="A54" s="21"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="11"/>
       <c r="D54" s="5" t="s">
         <v>35</v>
       </c>
@@ -1833,9 +1854,9 @@
       <c r="F54" s="18"/>
     </row>
     <row r="55" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="11"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="10"/>
+      <c r="A55" s="21"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="16"/>
       <c r="D55" s="6" t="s">
         <v>37</v>
       </c>
@@ -1845,11 +1866,11 @@
       <c r="F55" s="19"/>
     </row>
     <row r="56" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="11"/>
-      <c r="B56" s="14" t="s">
+      <c r="A56" s="21"/>
+      <c r="B56" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="15" t="s">
         <v>71</v>
       </c>
       <c r="D56" s="4" t="s">
@@ -1863,9 +1884,9 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="11"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="9"/>
+      <c r="A57" s="21"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="11"/>
       <c r="D57" s="5" t="s">
         <v>23</v>
       </c>
@@ -1875,9 +1896,9 @@
       <c r="F57" s="18"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="11"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="9"/>
+      <c r="A58" s="21"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="11"/>
       <c r="D58" s="5" t="s">
         <v>24</v>
       </c>
@@ -1887,31 +1908,31 @@
       <c r="F58" s="18"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="11"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="9"/>
+      <c r="A59" s="21"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="11"/>
       <c r="D59" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E59" s="11" t="s">
         <v>63</v>
       </c>
       <c r="F59" s="18"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
-      <c r="B60" s="15"/>
-      <c r="C60" s="9"/>
+      <c r="A60" s="21"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="11"/>
       <c r="D60" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E60" s="9"/>
+      <c r="E60" s="11"/>
       <c r="F60" s="18"/>
     </row>
     <row r="61" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="11"/>
-      <c r="B61" s="15"/>
-      <c r="C61" s="9"/>
+      <c r="A61" s="21"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="11"/>
       <c r="D61" s="5" t="s">
         <v>75</v>
       </c>
@@ -1921,9 +1942,9 @@
       <c r="F61" s="18"/>
     </row>
     <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="11"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="9"/>
+      <c r="A62" s="21"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="11"/>
       <c r="D62" s="5" t="s">
         <v>73</v>
       </c>
@@ -1933,9 +1954,9 @@
       <c r="F62" s="18"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" s="11"/>
-      <c r="B63" s="15"/>
-      <c r="C63" s="9"/>
+      <c r="A63" s="21"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="11"/>
       <c r="D63" s="5" t="s">
         <v>65</v>
       </c>
@@ -1945,9 +1966,9 @@
       <c r="F63" s="18"/>
     </row>
     <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="11"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="9"/>
+      <c r="A64" s="21"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="11"/>
       <c r="D64" s="5" t="s">
         <v>67</v>
       </c>
@@ -1957,9 +1978,9 @@
       <c r="F64" s="18"/>
     </row>
     <row r="65" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="11"/>
-      <c r="B65" s="15"/>
-      <c r="C65" s="9"/>
+      <c r="A65" s="21"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="11"/>
       <c r="D65" s="5" t="s">
         <v>35</v>
       </c>
@@ -1969,9 +1990,9 @@
       <c r="F65" s="18"/>
     </row>
     <row r="66" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="11"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="10"/>
+      <c r="A66" s="21"/>
+      <c r="B66" s="14"/>
+      <c r="C66" s="16"/>
       <c r="D66" s="6" t="s">
         <v>37</v>
       </c>
@@ -1981,11 +2002,11 @@
       <c r="F66" s="19"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="11"/>
-      <c r="B67" s="14" t="s">
+      <c r="A67" s="21"/>
+      <c r="B67" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="15" t="s">
         <v>76</v>
       </c>
       <c r="D67" s="4" t="s">
@@ -1999,9 +2020,9 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="11"/>
-      <c r="B68" s="15"/>
-      <c r="C68" s="9"/>
+      <c r="A68" s="21"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="11"/>
       <c r="D68" s="5" t="s">
         <v>23</v>
       </c>
@@ -2011,9 +2032,9 @@
       <c r="F68" s="18"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="11"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="9"/>
+      <c r="A69" s="21"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="11"/>
       <c r="D69" s="5" t="s">
         <v>24</v>
       </c>
@@ -2023,31 +2044,31 @@
       <c r="F69" s="18"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="11"/>
-      <c r="B70" s="15"/>
-      <c r="C70" s="9"/>
+      <c r="A70" s="21"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="11"/>
       <c r="D70" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E70" s="9" t="s">
+      <c r="E70" s="11" t="s">
         <v>63</v>
       </c>
       <c r="F70" s="18"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="11"/>
-      <c r="B71" s="15"/>
-      <c r="C71" s="9"/>
+      <c r="A71" s="21"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="11"/>
       <c r="D71" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E71" s="9"/>
+      <c r="E71" s="11"/>
       <c r="F71" s="18"/>
     </row>
     <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
-      <c r="B72" s="15"/>
-      <c r="C72" s="9"/>
+      <c r="A72" s="21"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="11"/>
       <c r="D72" s="5" t="s">
         <v>78</v>
       </c>
@@ -2057,9 +2078,9 @@
       <c r="F72" s="18"/>
     </row>
     <row r="73" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="11"/>
-      <c r="B73" s="15"/>
-      <c r="C73" s="9"/>
+      <c r="A73" s="21"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="11"/>
       <c r="D73" s="5" t="s">
         <v>73</v>
       </c>
@@ -2069,9 +2090,9 @@
       <c r="F73" s="18"/>
     </row>
     <row r="74" spans="1:6" ht="165" x14ac:dyDescent="0.25">
-      <c r="A74" s="11"/>
-      <c r="B74" s="15"/>
-      <c r="C74" s="9"/>
+      <c r="A74" s="21"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="11"/>
       <c r="D74" s="5" t="s">
         <v>77</v>
       </c>
@@ -2081,9 +2102,9 @@
       <c r="F74" s="18"/>
     </row>
     <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="11"/>
-      <c r="B75" s="15"/>
-      <c r="C75" s="9"/>
+      <c r="A75" s="21"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="11"/>
       <c r="D75" s="5" t="s">
         <v>67</v>
       </c>
@@ -2093,9 +2114,9 @@
       <c r="F75" s="18"/>
     </row>
     <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="11"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="9"/>
+      <c r="A76" s="21"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="11"/>
       <c r="D76" s="5" t="s">
         <v>35</v>
       </c>
@@ -2105,9 +2126,9 @@
       <c r="F76" s="18"/>
     </row>
     <row r="77" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="11"/>
-      <c r="B77" s="16"/>
-      <c r="C77" s="10"/>
+      <c r="A77" s="21"/>
+      <c r="B77" s="14"/>
+      <c r="C77" s="16"/>
       <c r="D77" s="6" t="s">
         <v>37</v>
       </c>
@@ -2116,672 +2137,805 @@
       </c>
       <c r="F77" s="19"/>
     </row>
+    <row r="78" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F78" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="9"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E79" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F79" s="18"/>
+    </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C80" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C81" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C82" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="B84" s="14" t="s">
+      <c r="A80" s="9"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E80" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F80" s="18"/>
+    </row>
+    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="9"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E81" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F81" s="18"/>
+    </row>
+    <row r="82" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="9"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F82" s="18"/>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="9"/>
+      <c r="B83" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C83" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="C84" s="8" t="s">
+      <c r="D83" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F83" s="18"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="9"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F84" s="18"/>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="9"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D84" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E84" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F84" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
-      <c r="B85" s="15"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="E85" s="5" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="F85" s="18"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
-      <c r="B86" s="15"/>
-      <c r="C86" s="9"/>
+    <row r="86" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A86" s="9"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="11"/>
       <c r="D86" s="5" t="s">
         <v>88</v>
       </c>
       <c r="E86" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F86" s="18"/>
+    </row>
+    <row r="87" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="10"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="16"/>
+      <c r="D87" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="F86" s="18"/>
-    </row>
-    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="11"/>
-      <c r="B87" s="15"/>
-      <c r="C87" s="9"/>
-      <c r="D87" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E87" s="5" t="s">
+      <c r="E87" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F87" s="18"/>
-    </row>
-    <row r="88" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="11"/>
-      <c r="B88" s="16"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E88" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F88" s="19"/>
+      <c r="F87" s="19"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F88" s="20" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="11"/>
-      <c r="B89" s="14" t="s">
+      <c r="A89" s="9"/>
+      <c r="B89" s="13"/>
+      <c r="C89" s="11"/>
+      <c r="D89" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F89" s="21"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="9"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="11"/>
+      <c r="D90" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E90" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C89" s="8" t="s">
+      <c r="F90" s="21"/>
+    </row>
+    <row r="91" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A91" s="9"/>
+      <c r="B91" s="13"/>
+      <c r="C91" s="11"/>
+      <c r="D91" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="D89" s="4" t="s">
+      <c r="E91" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F91" s="21"/>
+    </row>
+    <row r="92" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A92" s="9"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="11"/>
+      <c r="D92" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F92" s="21"/>
+    </row>
+    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A93" s="9"/>
+      <c r="B93" s="13"/>
+      <c r="C93" s="11"/>
+      <c r="D93" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F93" s="21"/>
+    </row>
+    <row r="94" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="9"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="16"/>
+      <c r="D94" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F94" s="22"/>
+    </row>
+    <row r="95" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="9"/>
+      <c r="B95" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D95" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E89" s="4" t="s">
+      <c r="E95" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F89" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="11"/>
-      <c r="B90" s="15"/>
-      <c r="C90" s="9"/>
-      <c r="D90" s="5" t="s">
+      <c r="F95" s="20" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="9"/>
+      <c r="B96" s="13"/>
+      <c r="C96" s="11"/>
+      <c r="D96" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E90" s="5" t="s">
+      <c r="E96" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F90" s="18"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" s="11"/>
-      <c r="B91" s="15"/>
-      <c r="C91" s="9"/>
-      <c r="D91" s="5" t="s">
+      <c r="F96" s="21"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="9"/>
+      <c r="B97" s="13"/>
+      <c r="C97" s="11"/>
+      <c r="D97" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E91" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="F91" s="18"/>
-    </row>
-    <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="11"/>
-      <c r="B92" s="15"/>
-      <c r="C92" s="9"/>
-      <c r="D92" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="E92" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="F92" s="18"/>
-    </row>
-    <row r="93" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="11"/>
-      <c r="B93" s="16"/>
-      <c r="C93" s="10"/>
-      <c r="D93" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="E93" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F93" s="19"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B94" s="14" t="s">
+      <c r="E97" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F97" s="21"/>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="9"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="11"/>
+      <c r="D98" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F98" s="21"/>
+    </row>
+    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="9"/>
+      <c r="B99" s="13"/>
+      <c r="C99" s="11"/>
+      <c r="D99" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F99" s="21"/>
+    </row>
+    <row r="100" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A100" s="9"/>
+      <c r="B100" s="13"/>
+      <c r="C100" s="11"/>
+      <c r="D100" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E100" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F100" s="21"/>
+    </row>
+    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101" s="9"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="11"/>
+      <c r="D101" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E101" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F101" s="21"/>
+    </row>
+    <row r="102" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="9"/>
+      <c r="B102" s="14"/>
+      <c r="C102" s="16"/>
+      <c r="D102" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F102" s="22"/>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="9"/>
+      <c r="B103" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F103" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="9"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="11"/>
+      <c r="D104" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E104" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F104" s="21"/>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="9"/>
+      <c r="B105" s="13"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E105" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F105" s="21"/>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="9"/>
+      <c r="B106" s="13"/>
+      <c r="C106" s="11"/>
+      <c r="D106" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F106" s="21"/>
+    </row>
+    <row r="107" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A107" s="9"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="11"/>
+      <c r="D107" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E107" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F107" s="21"/>
+    </row>
+    <row r="108" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A108" s="9"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="11"/>
+      <c r="D108" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F108" s="21"/>
+    </row>
+    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="9"/>
+      <c r="B109" s="13"/>
+      <c r="C109" s="11"/>
+      <c r="D109" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F109" s="21"/>
+    </row>
+    <row r="110" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="9"/>
+      <c r="B110" s="14"/>
+      <c r="C110" s="16"/>
+      <c r="D110" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E110" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F110" s="22"/>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="9"/>
+      <c r="B111" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="C94" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="D94" s="4" t="s">
+      <c r="C111" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D111" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E94" s="4" t="s">
+      <c r="E111" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F94" s="12" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="11"/>
-      <c r="B95" s="15"/>
-      <c r="C95" s="9"/>
-      <c r="D95" s="5" t="s">
+      <c r="F111" s="20" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="9"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="11"/>
+      <c r="D112" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E95" s="5" t="s">
+      <c r="E112" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F95" s="11"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="11"/>
-      <c r="B96" s="15"/>
-      <c r="C96" s="9"/>
-      <c r="D96" s="5" t="s">
+      <c r="F112" s="21"/>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="9"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="11"/>
+      <c r="D113" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F113" s="21"/>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="9"/>
+      <c r="B114" s="13"/>
+      <c r="C114" s="11"/>
+      <c r="D114" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F114" s="21"/>
+    </row>
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="9"/>
+      <c r="B115" s="13"/>
+      <c r="C115" s="11"/>
+      <c r="D115" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E115" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E96" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F96" s="11"/>
-    </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A97" s="11"/>
-      <c r="B97" s="15"/>
-      <c r="C97" s="9"/>
-      <c r="D97" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="E97" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F97" s="11"/>
-    </row>
-    <row r="98" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A98" s="11"/>
-      <c r="B98" s="15"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E98" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F98" s="11"/>
-    </row>
-    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A99" s="11"/>
-      <c r="B99" s="15"/>
-      <c r="C99" s="9"/>
-      <c r="D99" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E99" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="F99" s="11"/>
-    </row>
-    <row r="100" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="11"/>
-      <c r="B100" s="16"/>
-      <c r="C100" s="10"/>
-      <c r="D100" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F100" s="13"/>
-    </row>
-    <row r="101" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="11"/>
-      <c r="B101" s="14" t="s">
+      <c r="F115" s="21"/>
+    </row>
+    <row r="116" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A116" s="9"/>
+      <c r="B116" s="13"/>
+      <c r="C116" s="11"/>
+      <c r="D116" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E116" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F116" s="21"/>
+    </row>
+    <row r="117" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A117" s="9"/>
+      <c r="B117" s="13"/>
+      <c r="C117" s="11"/>
+      <c r="D117" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E117" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="F117" s="21"/>
+    </row>
+    <row r="118" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="9"/>
+      <c r="B118" s="14"/>
+      <c r="C118" s="16"/>
+      <c r="D118" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F118" s="22"/>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="9"/>
+      <c r="B119" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="C101" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D101" s="4" t="s">
+      <c r="C119" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="D119" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E101" s="4" t="s">
+      <c r="E119" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F101" s="12" t="s">
+      <c r="F119" s="20" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" s="11"/>
-      <c r="B102" s="15"/>
-      <c r="C102" s="9"/>
-      <c r="D102" s="5" t="s">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="9"/>
+      <c r="B120" s="13"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E102" s="5" t="s">
+      <c r="E120" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F102" s="11"/>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" s="11"/>
-      <c r="B103" s="15"/>
-      <c r="C103" s="9"/>
-      <c r="D103" s="5" t="s">
+      <c r="F120" s="21"/>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="9"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="11"/>
+      <c r="D121" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E121" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F121" s="21"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="9"/>
+      <c r="B122" s="13"/>
+      <c r="C122" s="11"/>
+      <c r="D122" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E122" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F122" s="21"/>
+    </row>
+    <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="9"/>
+      <c r="B123" s="13"/>
+      <c r="C123" s="11"/>
+      <c r="D123" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="E123" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="E103" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F103" s="11"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" s="11"/>
-      <c r="B104" s="15"/>
-      <c r="C104" s="9"/>
-      <c r="D104" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E104" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F104" s="11"/>
-    </row>
-    <row r="105" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="11"/>
-      <c r="B105" s="15"/>
-      <c r="C105" s="9"/>
-      <c r="D105" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E105" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F105" s="11"/>
-    </row>
-    <row r="106" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A106" s="11"/>
-      <c r="B106" s="15"/>
-      <c r="C106" s="9"/>
-      <c r="D106" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E106" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F106" s="11"/>
-    </row>
-    <row r="107" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A107" s="11"/>
-      <c r="B107" s="15"/>
-      <c r="C107" s="9"/>
-      <c r="D107" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="E107" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F107" s="11"/>
-    </row>
-    <row r="108" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="11"/>
-      <c r="B108" s="16"/>
-      <c r="C108" s="10"/>
-      <c r="D108" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="F108" s="13"/>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" s="11"/>
-      <c r="B109" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="C109" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D109" s="4" t="s">
+      <c r="F123" s="21"/>
+    </row>
+    <row r="124" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A124" s="9"/>
+      <c r="B124" s="13"/>
+      <c r="C124" s="11"/>
+      <c r="D124" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E124" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F124" s="21"/>
+    </row>
+    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="9"/>
+      <c r="B125" s="13"/>
+      <c r="C125" s="11"/>
+      <c r="D125" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E125" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F125" s="21"/>
+    </row>
+    <row r="126" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="10"/>
+      <c r="B126" s="14"/>
+      <c r="C126" s="16"/>
+      <c r="D126" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="F126" s="22"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="26" t="s">
+        <v>169</v>
+      </c>
+      <c r="B127" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C127" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D127" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E109" s="4" t="s">
+      <c r="E127" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F109" s="12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" s="11"/>
-      <c r="B110" s="15"/>
-      <c r="C110" s="9"/>
-      <c r="D110" s="5" t="s">
+      <c r="F127" s="20" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="27"/>
+      <c r="B128" s="13"/>
+      <c r="C128" s="11"/>
+      <c r="D128" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E110" s="5" t="s">
+      <c r="E128" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F110" s="11"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" s="11"/>
-      <c r="B111" s="15"/>
-      <c r="C111" s="9"/>
-      <c r="D111" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E111" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F111" s="11"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" s="11"/>
-      <c r="B112" s="15"/>
-      <c r="C112" s="9"/>
-      <c r="D112" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E112" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F112" s="11"/>
-    </row>
-    <row r="113" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="11"/>
-      <c r="B113" s="15"/>
-      <c r="C113" s="9"/>
-      <c r="D113" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E113" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F113" s="11"/>
-    </row>
-    <row r="114" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A114" s="11"/>
-      <c r="B114" s="15"/>
-      <c r="C114" s="9"/>
-      <c r="D114" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E114" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F114" s="11"/>
-    </row>
-    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A115" s="11"/>
-      <c r="B115" s="15"/>
-      <c r="C115" s="9"/>
-      <c r="D115" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E115" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F115" s="11"/>
-    </row>
-    <row r="116" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="11"/>
-      <c r="B116" s="16"/>
-      <c r="C116" s="10"/>
-      <c r="D116" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E116" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="F116" s="13"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="11"/>
-      <c r="B117" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="D117" s="4" t="s">
+      <c r="F128" s="21"/>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="27"/>
+      <c r="B129" s="13"/>
+      <c r="C129" s="11"/>
+      <c r="D129" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E129" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F129" s="21"/>
+    </row>
+    <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A130" s="27"/>
+      <c r="B130" s="13"/>
+      <c r="C130" s="11"/>
+      <c r="D130" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E130" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F130" s="21"/>
+    </row>
+    <row r="131" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="27"/>
+      <c r="B131" s="14"/>
+      <c r="C131" s="16"/>
+      <c r="D131" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F131" s="21"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="27"/>
+      <c r="B132" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C132" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D132" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E117" s="4" t="s">
+      <c r="E132" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F117" s="12" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="11"/>
-      <c r="B118" s="15"/>
-      <c r="C118" s="9"/>
-      <c r="D118" s="5" t="s">
+      <c r="F132" s="21"/>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="27"/>
+      <c r="B133" s="13"/>
+      <c r="C133" s="11"/>
+      <c r="D133" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E118" s="5" t="s">
+      <c r="E133" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F118" s="11"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" s="11"/>
-      <c r="B119" s="15"/>
-      <c r="C119" s="9"/>
-      <c r="D119" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E119" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F119" s="11"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" s="11"/>
-      <c r="B120" s="15"/>
-      <c r="C120" s="9"/>
-      <c r="D120" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E120" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F120" s="11"/>
-    </row>
-    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A121" s="11"/>
-      <c r="B121" s="15"/>
-      <c r="C121" s="9"/>
-      <c r="D121" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="E121" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F121" s="11"/>
-    </row>
-    <row r="122" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A122" s="11"/>
-      <c r="B122" s="15"/>
-      <c r="C122" s="9"/>
-      <c r="D122" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="E122" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F122" s="11"/>
-    </row>
-    <row r="123" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A123" s="11"/>
-      <c r="B123" s="15"/>
-      <c r="C123" s="9"/>
-      <c r="D123" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E123" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F123" s="11"/>
-    </row>
-    <row r="124" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="11"/>
-      <c r="B124" s="16"/>
-      <c r="C124" s="10"/>
-      <c r="D124" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="E124" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F124" s="13"/>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" s="11"/>
-      <c r="B125" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="C125" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D125" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E125" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F125" s="12" t="s">
+      <c r="F133" s="21"/>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="27"/>
+      <c r="B134" s="13"/>
+      <c r="C134" s="11"/>
+      <c r="D134" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E134" s="5" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="11"/>
-      <c r="B126" s="15"/>
-      <c r="C126" s="9"/>
-      <c r="D126" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E126" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F126" s="11"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="11"/>
-      <c r="B127" s="15"/>
-      <c r="C127" s="9"/>
-      <c r="D127" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E127" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F127" s="11"/>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" s="11"/>
-      <c r="B128" s="15"/>
-      <c r="C128" s="9"/>
-      <c r="D128" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E128" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F128" s="11"/>
-    </row>
-    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A129" s="11"/>
-      <c r="B129" s="15"/>
-      <c r="C129" s="9"/>
-      <c r="D129" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="E129" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F129" s="11"/>
-    </row>
-    <row r="130" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A130" s="11"/>
-      <c r="B130" s="15"/>
-      <c r="C130" s="9"/>
-      <c r="D130" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E130" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="F130" s="11"/>
-    </row>
-    <row r="131" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A131" s="11"/>
-      <c r="B131" s="15"/>
-      <c r="C131" s="9"/>
-      <c r="D131" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E131" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F131" s="11"/>
-    </row>
-    <row r="132" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="11"/>
-      <c r="B132" s="16"/>
-      <c r="C132" s="10"/>
-      <c r="D132" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="E132" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="F132" s="13"/>
+      <c r="F134" s="21"/>
+    </row>
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A135" s="27"/>
+      <c r="B135" s="13"/>
+      <c r="C135" s="11"/>
+      <c r="D135" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E135" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F135" s="21"/>
+    </row>
+    <row r="136" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="28"/>
+      <c r="B136" s="14"/>
+      <c r="C136" s="16"/>
+      <c r="D136" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="E136" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F136" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="A25:A45"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="B46:B55"/>
-    <mergeCell ref="C46:C55"/>
-    <mergeCell ref="F46:F55"/>
-    <mergeCell ref="B35:B45"/>
-    <mergeCell ref="C35:C45"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F35:F45"/>
-    <mergeCell ref="A46:A77"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F56:F66"/>
-    <mergeCell ref="C56:C66"/>
-    <mergeCell ref="B56:B66"/>
+  <mergeCells count="63">
+    <mergeCell ref="A127:A136"/>
+    <mergeCell ref="F78:F87"/>
+    <mergeCell ref="B127:B131"/>
+    <mergeCell ref="C127:C131"/>
+    <mergeCell ref="C132:C136"/>
+    <mergeCell ref="B132:B136"/>
+    <mergeCell ref="F127:F136"/>
+    <mergeCell ref="A78:A87"/>
+    <mergeCell ref="A88:A126"/>
+    <mergeCell ref="F119:F126"/>
+    <mergeCell ref="C119:C126"/>
+    <mergeCell ref="C111:C118"/>
+    <mergeCell ref="C103:C110"/>
+    <mergeCell ref="C95:C102"/>
+    <mergeCell ref="F88:F94"/>
+    <mergeCell ref="F95:F102"/>
+    <mergeCell ref="F103:F110"/>
+    <mergeCell ref="F111:F118"/>
+    <mergeCell ref="B88:B94"/>
+    <mergeCell ref="B95:B102"/>
+    <mergeCell ref="B103:B110"/>
+    <mergeCell ref="B111:B118"/>
+    <mergeCell ref="B119:B126"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="C78:C82"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="B83:B87"/>
+    <mergeCell ref="C83:C87"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F67:F77"/>
+    <mergeCell ref="C67:C77"/>
+    <mergeCell ref="B67:B77"/>
+    <mergeCell ref="C88:C94"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="E28:E29"/>
     <mergeCell ref="F25:F34"/>
@@ -2798,34 +2952,20 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F8:F15"/>
     <mergeCell ref="C8:C15"/>
-    <mergeCell ref="B125:B132"/>
-    <mergeCell ref="B8:B15"/>
-    <mergeCell ref="F84:F88"/>
-    <mergeCell ref="C84:C88"/>
-    <mergeCell ref="B84:B88"/>
-    <mergeCell ref="F89:F93"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="C89:C93"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F67:F77"/>
-    <mergeCell ref="C67:C77"/>
-    <mergeCell ref="B67:B77"/>
-    <mergeCell ref="C94:C100"/>
-    <mergeCell ref="A84:A93"/>
-    <mergeCell ref="A94:A132"/>
-    <mergeCell ref="F125:F132"/>
-    <mergeCell ref="C125:C132"/>
-    <mergeCell ref="C117:C124"/>
-    <mergeCell ref="C109:C116"/>
-    <mergeCell ref="C101:C108"/>
-    <mergeCell ref="F94:F100"/>
-    <mergeCell ref="F101:F108"/>
-    <mergeCell ref="F109:F116"/>
-    <mergeCell ref="F117:F124"/>
-    <mergeCell ref="B94:B100"/>
-    <mergeCell ref="B101:B108"/>
-    <mergeCell ref="B109:B116"/>
-    <mergeCell ref="B117:B124"/>
+    <mergeCell ref="A25:A45"/>
+    <mergeCell ref="E49:E50"/>
+    <mergeCell ref="B46:B55"/>
+    <mergeCell ref="C46:C55"/>
+    <mergeCell ref="F46:F55"/>
+    <mergeCell ref="B35:B45"/>
+    <mergeCell ref="C35:C45"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F35:F45"/>
+    <mergeCell ref="A46:A77"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F56:F66"/>
+    <mergeCell ref="C56:C66"/>
+    <mergeCell ref="B56:B66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>